<commit_message>
Data Insert working propertly - Fix Extra Row
</commit_message>
<xml_diff>
--- a/Python_Tests/src/Prueba.xlsx
+++ b/Python_Tests/src/Prueba.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -443,7 +443,22 @@
           <t>EC20230804</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>EC20230804</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00218
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
         <is>
           <t xml:space="preserve">00218
 </t>

</xml_diff>

<commit_message>
Excel Working - 60 Fix
</commit_message>
<xml_diff>
--- a/Python_Tests/src/Prueba.xlsx
+++ b/Python_Tests/src/Prueba.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -24,16 +24,30 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,12 +55,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,28 +444,49 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="7.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="12.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="7.140625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="7.7109375" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="7" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="5.28515625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Campo1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Campo2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Campo3</t>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tag20</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tag25</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tag28C</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tag60F</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Tag61</t>
         </is>
       </c>
     </row>
@@ -449,32 +502,83 @@
 </t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4053879706
+</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>00216</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">00001
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>210803</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>MXN</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>000000264505,15</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>EC20220804</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">00217
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>210803</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0803</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>000000002323,02</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NTRF</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000225924//5209
 </t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>EC20230804</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">00218
-</t>
-        </is>
-      </c>
+      <c r="P3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>